<commit_message>
Updated Prioritization and Grammar Naziing
GN in Use Case Diagram
</commit_message>
<xml_diff>
--- a/System development files/Prioritization.xlsx
+++ b/System development files/Prioritization.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Action</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>Create reservation</t>
-  </si>
-  <si>
     <t>Find reservation</t>
   </si>
   <si>
@@ -53,6 +50,117 @@
   </si>
   <si>
     <t>Delete merchandise</t>
+  </si>
+  <si>
+    <t>Make reservation</t>
+  </si>
+  <si>
+    <t>Create table</t>
+  </si>
+  <si>
+    <t>Find table</t>
+  </si>
+  <si>
+    <t>Update table</t>
+  </si>
+  <si>
+    <t>delete table</t>
+  </si>
+  <si>
+    <t>Create preorder</t>
+  </si>
+  <si>
+    <t>Update preorder</t>
+  </si>
+  <si>
+    <t>Find preorder</t>
+  </si>
+  <si>
+    <t>Delete preorder</t>
+  </si>
+  <si>
+    <t>Make order</t>
+  </si>
+  <si>
+    <t>Update order</t>
+  </si>
+  <si>
+    <t>Find order</t>
+  </si>
+  <si>
+    <t>Cancel order</t>
+  </si>
+  <si>
+    <t>Make payment</t>
+  </si>
+  <si>
+    <t>Add discount</t>
+  </si>
+  <si>
+    <t>Send notification to waiters</t>
+  </si>
+  <si>
+    <t>Send notification to chef</t>
+  </si>
+  <si>
+    <t>Process notification</t>
+  </si>
+  <si>
+    <t>Create event</t>
+  </si>
+  <si>
+    <t>Customer check-in</t>
+  </si>
+  <si>
+    <t>Update event</t>
+  </si>
+  <si>
+    <t>Find event</t>
+  </si>
+  <si>
+    <t>Delete event</t>
+  </si>
+  <si>
+    <t>Create supplier</t>
+  </si>
+  <si>
+    <t>Update supplier</t>
+  </si>
+  <si>
+    <t>Find supplier</t>
+  </si>
+  <si>
+    <t>Delete supplier</t>
+  </si>
+  <si>
+    <t>Create course</t>
+  </si>
+  <si>
+    <t>Update course</t>
+  </si>
+  <si>
+    <t>Find course</t>
+  </si>
+  <si>
+    <t>Delete course</t>
+  </si>
+  <si>
+    <t>Create staff</t>
+  </si>
+  <si>
+    <t>Update staff</t>
+  </si>
+  <si>
+    <t>Find staff</t>
+  </si>
+  <si>
+    <t>Delete staff</t>
+  </si>
+  <si>
+    <t>Get statistics</t>
+  </si>
+  <si>
+    <t>Get supply statistics</t>
   </si>
 </sst>
 </file>
@@ -68,12 +176,72 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,8 +256,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -394,15 +572,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F9"/>
+  <dimension ref="B1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -426,8 +604,8 @@
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>9</v>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -439,10 +617,13 @@
         <f>C2*D2</f>
         <v>20</v>
       </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -451,98 +632,767 @@
         <v>5</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E9" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E45" si="0">C3*D3</f>
         <v>25</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="F19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F26">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F27">
         <v>11</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F28">
         <v>12</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>1</v>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F37">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F40">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F41">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F42">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F45">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>